<commit_message>
doc processing and eems upload
</commit_message>
<xml_diff>
--- a/Data/DOC/20231002_Readme_NPOC_TN_COMPASS_TEMPEST_EXP_Run2.xlsx
+++ b/Data/DOC/20231002_Readme_NPOC_TN_COMPASS_TEMPEST_EXP_Run2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oten406/Library/CloudStorage/OneDrive-PNNL/Desktop/Synoptic NPOC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/tempest_ionic_strength/Data/DOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DED3DA9E-7BBD-C846-8FAC-65B913DEB63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5387A4C1-B96C-9540-8298-1451EA17AA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-440" yWindow="980" windowWidth="27640" windowHeight="15740" xr2:uid="{23205A7A-8F65-A549-9F74-05A3844C163E}"/>
+    <workbookView xWindow="1680" yWindow="780" windowWidth="27640" windowHeight="15740" xr2:uid="{23205A7A-8F65-A549-9F74-05A3844C163E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="110">
   <si>
     <t>Sample Name</t>
   </si>
@@ -408,9 +408,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -729,7 +728,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,6 +853,9 @@
       <c r="B11">
         <v>25</v>
       </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -956,6 +958,9 @@
       <c r="B23">
         <v>37</v>
       </c>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1012,6 +1017,9 @@
       <c r="B30">
         <v>44</v>
       </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1270,6 +1278,9 @@
       <c r="B60">
         <v>74</v>
       </c>
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -1375,36 +1386,36 @@
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
         <v>85</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72">
         <v>86</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
         <v>87</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1418,7 +1429,7 @@
       <c r="C74" t="s">
         <v>107</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1446,7 +1457,7 @@
       <c r="C76" t="s">
         <v>107</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="1" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>